<commit_message>
Add final scoring system with opening year and renovation analysis
- Removed brand penalties as requested
- Added opening year scoring (newer hotels get more points - max 5 pts)
- Added last renovation scoring (recent renovations get more points - max 5 pts)
- Corrected total keys to include rooms + suites + apartments
- Fixed room mix calculation (R+S+A properly detected)
- All star ratings now showing correctly
- All meeting space and facility data extracted properly
- All hotels have sauna (1 point each)

Analysis reveals GP Movenpick Media City leads due to:
- TripAdvisor rating 4.9 vs 4.0 (+10 points advantage)
- Superior meeting facilities (1150 sqm, 10 rooms)
- Newer opening year (2019 vs 2007)

Final scores: GP Movenpick 100/100, Grand Millennium Dubai 92.4/100

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Compset_Analysis_With_ML_Features_Final.xlsx
+++ b/Compset_Analysis_With_ML_Features_Final.xlsx
@@ -6,8 +6,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Features" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ML Features &amp; Scoring" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Points &amp; Scoring" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Features" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ML Features &amp; Scoring" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="181029" fullCalcOnLoad="1"/>
@@ -16,11 +17,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="22">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -103,8 +105,40 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <sz val="9"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="18">
     <fill>
       <patternFill/>
     </fill>
@@ -177,8 +211,38 @@
         <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005B9BD5"/>
+        <bgColor rgb="005B9BD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+        <bgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6E0B4"/>
+        <bgColor rgb="00C6E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -216,11 +280,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -289,6 +359,126 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="15" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="12" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="16" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="15" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="12" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="17" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="16" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="15" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="12" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="17" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="16" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -653,6 +843,2096 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AE35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="10" customWidth="1" min="25" max="25"/>
+    <col width="10" customWidth="1" min="26" max="26"/>
+    <col width="10" customWidth="1" min="27" max="27"/>
+    <col width="10" customWidth="1" min="28" max="28"/>
+    <col width="10" customWidth="1" min="29" max="29"/>
+    <col width="10" customWidth="1" min="30" max="30"/>
+    <col width="10" customWidth="1" min="31" max="31"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="26" t="inlineStr">
+        <is>
+          <t>FINAL FEATURE POINTS &amp; SCORING (No Brand Penalty)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="27" t="inlineStr">
+        <is>
+          <t>Includes Opening Year &amp; Renovation Scoring</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="45" customHeight="1">
+      <c r="A4" s="41" t="inlineStr">
+        <is>
+          <t>Hotel</t>
+        </is>
+      </c>
+      <c r="B4" s="41" t="inlineStr">
+        <is>
+          <t>Star
+Rating</t>
+        </is>
+      </c>
+      <c r="C4" s="41" t="inlineStr">
+        <is>
+          <t>Star
+Multiplier</t>
+        </is>
+      </c>
+      <c r="D4" s="41" t="inlineStr">
+        <is>
+          <t>Room Mix
+(R/S/A)</t>
+        </is>
+      </c>
+      <c r="E4" s="41" t="inlineStr">
+        <is>
+          <t>Room Mix
+Points (3)</t>
+        </is>
+      </c>
+      <c r="F4" s="41" t="inlineStr">
+        <is>
+          <t>Total
+Keys</t>
+        </is>
+      </c>
+      <c r="G4" s="41" t="inlineStr">
+        <is>
+          <t>Total Keys
+Points (15)</t>
+        </is>
+      </c>
+      <c r="H4" s="41" t="inlineStr">
+        <is>
+          <t>Distance
+KM</t>
+        </is>
+      </c>
+      <c r="I4" s="41" t="inlineStr">
+        <is>
+          <t>Distance
+Points (20)</t>
+        </is>
+      </c>
+      <c r="J4" s="41" t="inlineStr">
+        <is>
+          <t>TripAdvisor
+Score</t>
+        </is>
+      </c>
+      <c r="K4" s="41" t="inlineStr">
+        <is>
+          <t>TripAdvisor
+Points (10)</t>
+        </is>
+      </c>
+      <c r="L4" s="41" t="inlineStr">
+        <is>
+          <t>Booking.com
+Score</t>
+        </is>
+      </c>
+      <c r="M4" s="41" t="inlineStr">
+        <is>
+          <t>Booking.com
+Points (10)</t>
+        </is>
+      </c>
+      <c r="N4" s="41" t="inlineStr">
+        <is>
+          <t>Meeting
+Sqm</t>
+        </is>
+      </c>
+      <c r="O4" s="41" t="inlineStr">
+        <is>
+          <t>Meeting
+Rooms</t>
+        </is>
+      </c>
+      <c r="P4" s="41" t="inlineStr">
+        <is>
+          <t>Meeting
+Points (12)</t>
+        </is>
+      </c>
+      <c r="Q4" s="41" t="inlineStr">
+        <is>
+          <t>F&amp;B
+Total</t>
+        </is>
+      </c>
+      <c r="R4" s="41" t="inlineStr">
+        <is>
+          <t>F&amp;B
+Points (8)</t>
+        </is>
+      </c>
+      <c r="S4" s="41" t="inlineStr">
+        <is>
+          <t>Opening
+Year</t>
+        </is>
+      </c>
+      <c r="T4" s="41" t="inlineStr">
+        <is>
+          <t>Opening
+Points (5)</t>
+        </is>
+      </c>
+      <c r="U4" s="41" t="inlineStr">
+        <is>
+          <t>Last
+Renovation</t>
+        </is>
+      </c>
+      <c r="V4" s="41" t="inlineStr">
+        <is>
+          <t>Renovation
+Points (5)</t>
+        </is>
+      </c>
+      <c r="W4" s="41" t="inlineStr">
+        <is>
+          <t>Pool
+(1/0)</t>
+        </is>
+      </c>
+      <c r="X4" s="41" t="inlineStr">
+        <is>
+          <t>Gym
+(1/0)</t>
+        </is>
+      </c>
+      <c r="Y4" s="41" t="inlineStr">
+        <is>
+          <t>Spa
+(1/0)</t>
+        </is>
+      </c>
+      <c r="Z4" s="41" t="inlineStr">
+        <is>
+          <t>Sauna
+(1/0)</t>
+        </is>
+      </c>
+      <c r="AA4" s="41" t="inlineStr">
+        <is>
+          <t>Kids Club
+(1/0)</t>
+        </is>
+      </c>
+      <c r="AB4" s="41" t="inlineStr">
+        <is>
+          <t>Base Total
+Points</t>
+        </is>
+      </c>
+      <c r="AC4" s="41" t="inlineStr">
+        <is>
+          <t>After Star
+Adjustment</t>
+        </is>
+      </c>
+      <c r="AD4" s="41" t="inlineStr">
+        <is>
+          <t>Final
+Points</t>
+        </is>
+      </c>
+      <c r="AE4" s="41" t="inlineStr">
+        <is>
+          <t>Normalized
+Score (0-100)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="57" t="inlineStr">
+        <is>
+          <t>Grand Plaza Movenpick Media City</t>
+        </is>
+      </c>
+      <c r="B5" s="58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="59" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D5" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E5" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="61" t="n">
+        <v>235</v>
+      </c>
+      <c r="G5" s="62" t="n">
+        <v>1.202830188679245</v>
+      </c>
+      <c r="H5" s="59" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I5" s="62" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="J5" s="63" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="K5" s="62" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" s="63" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="M5" s="62" t="n">
+        <v>10</v>
+      </c>
+      <c r="N5" s="61" t="n">
+        <v>1150</v>
+      </c>
+      <c r="O5" s="61" t="n">
+        <v>10</v>
+      </c>
+      <c r="P5" s="62" t="n">
+        <v>6.586449864498645</v>
+      </c>
+      <c r="Q5" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="R5" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="T5" s="62" t="n">
+        <v>4.0625</v>
+      </c>
+      <c r="U5" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="V5" s="62" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="W5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="64" t="n">
+        <v>55.98511338651123</v>
+      </c>
+      <c r="AC5" s="65" t="n">
+        <v>72.7806474024646</v>
+      </c>
+      <c r="AD5" s="66" t="n">
+        <v>72.7806474024646</v>
+      </c>
+      <c r="AE5" s="67" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="68" t="inlineStr">
+        <is>
+          <t>Grand Millennium Dubai</t>
+        </is>
+      </c>
+      <c r="B6" s="58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="59" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D6" s="58" t="inlineStr">
+        <is>
+          <t>R+S+A</t>
+        </is>
+      </c>
+      <c r="E6" s="60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="61" t="n">
+        <v>339</v>
+      </c>
+      <c r="G6" s="62" t="n">
+        <v>3.04245283018868</v>
+      </c>
+      <c r="H6" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="62" t="n">
+        <v>20</v>
+      </c>
+      <c r="J6" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="63" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="M6" s="62" t="n">
+        <v>9.333333333333336</v>
+      </c>
+      <c r="N6" s="61" t="n">
+        <v>315</v>
+      </c>
+      <c r="O6" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="P6" s="62" t="n">
+        <v>2.485853658536586</v>
+      </c>
+      <c r="Q6" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="R6" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="S6" s="61" t="n">
+        <v>2007</v>
+      </c>
+      <c r="T6" s="62" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="U6" s="61" t="n">
+        <v>2024</v>
+      </c>
+      <c r="V6" s="62" t="n">
+        <v>4.722222222222222</v>
+      </c>
+      <c r="W6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="64" t="n">
+        <v>52.89636204428082</v>
+      </c>
+      <c r="AC6" s="65" t="n">
+        <v>68.76527065756507</v>
+      </c>
+      <c r="AD6" s="66" t="n">
+        <v>68.76527065756507</v>
+      </c>
+      <c r="AE6" s="67" t="n">
+        <v>92.38530714109775</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="57" t="inlineStr">
+        <is>
+          <t>voco Bonnington Dubai</t>
+        </is>
+      </c>
+      <c r="B7" s="58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="59" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D7" s="58" t="inlineStr">
+        <is>
+          <t>S+A</t>
+        </is>
+      </c>
+      <c r="E7" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="61" t="n">
+        <v>480</v>
+      </c>
+      <c r="G7" s="62" t="n">
+        <v>5.536556603773585</v>
+      </c>
+      <c r="H7" s="59" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="I7" s="62" t="n">
+        <v>2.600000000000002</v>
+      </c>
+      <c r="J7" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K7" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="63" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="M7" s="62" t="n">
+        <v>2.666666666666665</v>
+      </c>
+      <c r="N7" s="61" t="n">
+        <v>640</v>
+      </c>
+      <c r="O7" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" s="62" t="n">
+        <v>3.735067750677507</v>
+      </c>
+      <c r="Q7" s="61" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="62" t="n">
+        <v>8</v>
+      </c>
+      <c r="S7" s="61" t="n">
+        <v>2022</v>
+      </c>
+      <c r="T7" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="U7" s="61" t="n">
+        <v>2022</v>
+      </c>
+      <c r="V7" s="62" t="n">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="W7" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="64" t="n">
+        <v>37.70495768778442</v>
+      </c>
+      <c r="AC7" s="65" t="n">
+        <v>49.01644499411975</v>
+      </c>
+      <c r="AD7" s="66" t="n">
+        <v>49.01644499411975</v>
+      </c>
+      <c r="AE7" s="67" t="n">
+        <v>54.93396663060592</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="57" t="inlineStr">
+        <is>
+          <t>Mercure Dubai Barsha Heights</t>
+        </is>
+      </c>
+      <c r="B8" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="58" t="inlineStr">
+        <is>
+          <t>S+A</t>
+        </is>
+      </c>
+      <c r="E8" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="61" t="n">
+        <v>1015</v>
+      </c>
+      <c r="G8" s="62" t="n">
+        <v>15</v>
+      </c>
+      <c r="H8" s="59" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="62" t="n">
+        <v>17</v>
+      </c>
+      <c r="J8" s="63" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K8" s="62" t="n">
+        <v>5.555555555555554</v>
+      </c>
+      <c r="L8" s="63" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="M8" s="62" t="n">
+        <v>3.333333333333329</v>
+      </c>
+      <c r="N8" s="61" t="n">
+        <v>446</v>
+      </c>
+      <c r="O8" s="61" t="n">
+        <v>8</v>
+      </c>
+      <c r="P8" s="62" t="n">
+        <v>3.213875338753388</v>
+      </c>
+      <c r="Q8" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="R8" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" s="61" t="n">
+        <v>2012</v>
+      </c>
+      <c r="T8" s="62" t="n">
+        <v>1.875</v>
+      </c>
+      <c r="U8" s="61" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V8" s="62" t="n">
+        <v>3.055555555555556</v>
+      </c>
+      <c r="W8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="64" t="n">
+        <v>61.03331978319783</v>
+      </c>
+      <c r="AC8" s="65" t="n">
+        <v>42.72332384823848</v>
+      </c>
+      <c r="AD8" s="66" t="n">
+        <v>42.72332384823848</v>
+      </c>
+      <c r="AE8" s="67" t="n">
+        <v>42.99979763622233</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="57" t="inlineStr">
+        <is>
+          <t>Pullman JLT</t>
+        </is>
+      </c>
+      <c r="B9" s="58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="59" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D9" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E9" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="61" t="n">
+        <v>354</v>
+      </c>
+      <c r="G9" s="62" t="n">
+        <v>3.307783018867924</v>
+      </c>
+      <c r="H9" s="59" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="I9" s="62" t="n">
+        <v>0.6000000000000005</v>
+      </c>
+      <c r="J9" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K9" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="63" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="M9" s="62" t="n">
+        <v>0.6666666666666647</v>
+      </c>
+      <c r="N9" s="61" t="n">
+        <v>550</v>
+      </c>
+      <c r="O9" s="61" t="n">
+        <v>11</v>
+      </c>
+      <c r="P9" s="62" t="n">
+        <v>4.144823848238483</v>
+      </c>
+      <c r="Q9" s="61" t="n">
+        <v>8</v>
+      </c>
+      <c r="R9" s="62" t="n">
+        <v>8</v>
+      </c>
+      <c r="S9" s="61" t="n">
+        <v>2014</v>
+      </c>
+      <c r="T9" s="62" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="U9" s="61" t="n">
+        <v>2025</v>
+      </c>
+      <c r="V9" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="W9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="64" t="n">
+        <v>31.21927353377307</v>
+      </c>
+      <c r="AC9" s="65" t="n">
+        <v>40.585055593905</v>
+      </c>
+      <c r="AD9" s="66" t="n">
+        <v>40.585055593905</v>
+      </c>
+      <c r="AE9" s="67" t="n">
+        <v>38.94482171712013</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="57" t="inlineStr">
+        <is>
+          <t>Millennium Place Barsha Heights</t>
+        </is>
+      </c>
+      <c r="B10" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D10" s="58" t="inlineStr">
+        <is>
+          <t>S+A</t>
+        </is>
+      </c>
+      <c r="E10" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="61" t="n">
+        <v>915</v>
+      </c>
+      <c r="G10" s="62" t="n">
+        <v>13.2311320754717</v>
+      </c>
+      <c r="H10" s="59" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="I10" s="62" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="J10" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K10" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="63" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="M10" s="62" t="n">
+        <v>4.000000000000005</v>
+      </c>
+      <c r="N10" s="61" t="n">
+        <v>146</v>
+      </c>
+      <c r="O10" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="P10" s="62" t="n">
+        <v>1.753062330623306</v>
+      </c>
+      <c r="Q10" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="R10" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="S10" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="T10" s="62" t="n">
+        <v>4.0625</v>
+      </c>
+      <c r="U10" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="V10" s="62" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="W10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="64" t="n">
+        <v>54.98002773942835</v>
+      </c>
+      <c r="AC10" s="65" t="n">
+        <v>38.48601941759984</v>
+      </c>
+      <c r="AD10" s="66" t="n">
+        <v>38.48601941759984</v>
+      </c>
+      <c r="AE10" s="67" t="n">
+        <v>34.96424485030654</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="57" t="inlineStr">
+        <is>
+          <t>Atana Hotel</t>
+        </is>
+      </c>
+      <c r="B11" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E11" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="61" t="n">
+        <v>828</v>
+      </c>
+      <c r="G11" s="62" t="n">
+        <v>11.69221698113208</v>
+      </c>
+      <c r="H11" s="59" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I11" s="62" t="n">
+        <v>19.72</v>
+      </c>
+      <c r="J11" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K11" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="63" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="M11" s="62" t="n">
+        <v>4.666666666666671</v>
+      </c>
+      <c r="N11" s="61" t="n">
+        <v>220</v>
+      </c>
+      <c r="O11" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="P11" s="62" t="n">
+        <v>1.913929539295393</v>
+      </c>
+      <c r="Q11" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="R11" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="S11" s="61" t="n">
+        <v>2015</v>
+      </c>
+      <c r="T11" s="62" t="n">
+        <v>2.8125</v>
+      </c>
+      <c r="U11" s="61" t="n">
+        <v>2017</v>
+      </c>
+      <c r="V11" s="62" t="n">
+        <v>2.777777777777778</v>
+      </c>
+      <c r="W11" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X11" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="64" t="n">
+        <v>54.58309096487192</v>
+      </c>
+      <c r="AC11" s="65" t="n">
+        <v>38.20816367541034</v>
+      </c>
+      <c r="AD11" s="66" t="n">
+        <v>38.20816367541034</v>
+      </c>
+      <c r="AE11" s="67" t="n">
+        <v>34.43732389860681</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="57" t="inlineStr">
+        <is>
+          <t>Two Seasons</t>
+        </is>
+      </c>
+      <c r="B12" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D12" s="58" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="61" t="n">
+        <v>1010</v>
+      </c>
+      <c r="G12" s="62" t="n">
+        <v>14.91155660377358</v>
+      </c>
+      <c r="H12" s="59" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I12" s="62" t="n">
+        <v>13</v>
+      </c>
+      <c r="J12" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="63" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="M12" s="62" t="n">
+        <v>4.000000000000005</v>
+      </c>
+      <c r="N12" s="61" t="n">
+        <v>1845</v>
+      </c>
+      <c r="O12" s="61" t="n">
+        <v>25</v>
+      </c>
+      <c r="P12" s="62" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="61" t="n">
+        <v>2009</v>
+      </c>
+      <c r="T12" s="62" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="U12" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="V12" s="62" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="W12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="64" t="n">
+        <v>53.18238993710693</v>
+      </c>
+      <c r="AC12" s="65" t="n">
+        <v>37.22767295597485</v>
+      </c>
+      <c r="AD12" s="66" t="n">
+        <v>37.22767295597485</v>
+      </c>
+      <c r="AE12" s="67" t="n">
+        <v>32.57793780513772</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="57" t="inlineStr">
+        <is>
+          <t>Taj JLT</t>
+        </is>
+      </c>
+      <c r="B13" s="58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="59" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D13" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E13" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="61" t="n">
+        <v>200</v>
+      </c>
+      <c r="G13" s="62" t="n">
+        <v>0.5837264150943396</v>
+      </c>
+      <c r="H13" s="59" t="n">
+        <v>10</v>
+      </c>
+      <c r="I13" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K13" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="63" t="n">
+        <v>9</v>
+      </c>
+      <c r="M13" s="62" t="n">
+        <v>8.66666666666667</v>
+      </c>
+      <c r="N13" s="61" t="n">
+        <v>335</v>
+      </c>
+      <c r="O13" s="61" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" s="62" t="n">
+        <v>1.932574525745257</v>
+      </c>
+      <c r="Q13" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="R13" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="S13" s="61" t="n">
+        <v>2017</v>
+      </c>
+      <c r="T13" s="62" t="n">
+        <v>3.4375</v>
+      </c>
+      <c r="U13" s="61" t="n">
+        <v>2017</v>
+      </c>
+      <c r="V13" s="62" t="n">
+        <v>2.777777777777778</v>
+      </c>
+      <c r="W13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="64" t="n">
+        <v>28.39824538528405</v>
+      </c>
+      <c r="AC13" s="65" t="n">
+        <v>36.91771900086926</v>
+      </c>
+      <c r="AD13" s="66" t="n">
+        <v>36.91771900086926</v>
+      </c>
+      <c r="AE13" s="67" t="n">
+        <v>31.99014634284741</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="57" t="inlineStr">
+        <is>
+          <t>TRYP by Wyndham Dubai</t>
+        </is>
+      </c>
+      <c r="B14" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D14" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E14" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="61" t="n">
+        <v>650</v>
+      </c>
+      <c r="G14" s="62" t="n">
+        <v>8.543632075471697</v>
+      </c>
+      <c r="H14" s="59" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="62" t="n">
+        <v>16</v>
+      </c>
+      <c r="J14" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K14" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="63" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="M14" s="62" t="n">
+        <v>6.666666666666665</v>
+      </c>
+      <c r="N14" s="61" t="n">
+        <v>357</v>
+      </c>
+      <c r="O14" s="61" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="62" t="n">
+        <v>1.867967479674797</v>
+      </c>
+      <c r="Q14" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="R14" s="62" t="n">
+        <v>5</v>
+      </c>
+      <c r="S14" s="61" t="n">
+        <v>2017</v>
+      </c>
+      <c r="T14" s="62" t="n">
+        <v>3.4375</v>
+      </c>
+      <c r="U14" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="V14" s="62" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="W14" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X14" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="64" t="n">
+        <v>50.84909955514649</v>
+      </c>
+      <c r="AC14" s="65" t="n">
+        <v>35.59436968860254</v>
+      </c>
+      <c r="AD14" s="66" t="n">
+        <v>35.59436968860254</v>
+      </c>
+      <c r="AE14" s="67" t="n">
+        <v>29.48056898606498</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="57" t="inlineStr">
+        <is>
+          <t>Mövenpick JLT</t>
+        </is>
+      </c>
+      <c r="B15" s="58" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="59" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D15" s="58" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E15" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="61" t="n">
+        <v>168</v>
+      </c>
+      <c r="G15" s="62" t="n">
+        <v>0.01768867924528302</v>
+      </c>
+      <c r="H15" s="59" t="n">
+        <v>10</v>
+      </c>
+      <c r="I15" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="63" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K15" s="62" t="n">
+        <v>5.555555555555554</v>
+      </c>
+      <c r="L15" s="63" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="M15" s="62" t="n">
+        <v>4.666666666666671</v>
+      </c>
+      <c r="N15" s="61" t="n">
+        <v>230</v>
+      </c>
+      <c r="O15" s="61" t="n">
+        <v>9</v>
+      </c>
+      <c r="P15" s="62" t="n">
+        <v>2.437289972899729</v>
+      </c>
+      <c r="Q15" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="R15" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="S15" s="61" t="n">
+        <v>2013</v>
+      </c>
+      <c r="T15" s="62" t="n">
+        <v>2.1875</v>
+      </c>
+      <c r="U15" s="61" t="n">
+        <v>2011</v>
+      </c>
+      <c r="V15" s="62" t="n">
+        <v>1.111111111111111</v>
+      </c>
+      <c r="W15" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X15" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="64" t="n">
+        <v>25.97581198547835</v>
+      </c>
+      <c r="AC15" s="65" t="n">
+        <v>33.76855558112185</v>
+      </c>
+      <c r="AD15" s="66" t="n">
+        <v>33.76855558112185</v>
+      </c>
+      <c r="AE15" s="67" t="n">
+        <v>26.01812585079099</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="57" t="inlineStr">
+        <is>
+          <t>Zabeel House The Greens</t>
+        </is>
+      </c>
+      <c r="B16" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D16" s="58" t="inlineStr">
+        <is>
+          <t>R+S+A</t>
+        </is>
+      </c>
+      <c r="E16" s="60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" s="61" t="n">
+        <v>210</v>
+      </c>
+      <c r="G16" s="62" t="n">
+        <v>0.7606132075471699</v>
+      </c>
+      <c r="H16" s="59" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="I16" s="62" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="J16" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K16" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="63" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="M16" s="62" t="n">
+        <v>8.000000000000005</v>
+      </c>
+      <c r="N16" s="61" t="n">
+        <v>156</v>
+      </c>
+      <c r="O16" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="P16" s="62" t="n">
+        <v>1.316422764227642</v>
+      </c>
+      <c r="Q16" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="R16" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="S16" s="61" t="n">
+        <v>2018</v>
+      </c>
+      <c r="T16" s="62" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="U16" s="61" t="n">
+        <v>2022</v>
+      </c>
+      <c r="V16" s="62" t="n">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="W16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="64" t="n">
+        <v>44.59370263844148</v>
+      </c>
+      <c r="AC16" s="65" t="n">
+        <v>31.21559184690903</v>
+      </c>
+      <c r="AD16" s="66" t="n">
+        <v>31.21559184690903</v>
+      </c>
+      <c r="AE16" s="67" t="n">
+        <v>21.17672840517391</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="57" t="inlineStr">
+        <is>
+          <t>Novotel Dubai Al Barsha</t>
+        </is>
+      </c>
+      <c r="B17" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D17" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E17" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="61" t="n">
+        <v>465</v>
+      </c>
+      <c r="G17" s="62" t="n">
+        <v>5.27122641509434</v>
+      </c>
+      <c r="H17" s="59" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="I17" s="62" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="J17" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K17" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="63" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="M17" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="61" t="n">
+        <v>1800</v>
+      </c>
+      <c r="O17" s="61" t="n">
+        <v>10</v>
+      </c>
+      <c r="P17" s="62" t="n">
+        <v>9.404878048780487</v>
+      </c>
+      <c r="Q17" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="R17" s="62" t="n">
+        <v>6</v>
+      </c>
+      <c r="S17" s="61" t="n">
+        <v>2013</v>
+      </c>
+      <c r="T17" s="62" t="n">
+        <v>2.1875</v>
+      </c>
+      <c r="U17" s="61" t="n">
+        <v>2012</v>
+      </c>
+      <c r="V17" s="62" t="n">
+        <v>1.388888888888889</v>
+      </c>
+      <c r="W17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="64" t="n">
+        <v>42.45249335276371</v>
+      </c>
+      <c r="AC17" s="65" t="n">
+        <v>29.71674534693459</v>
+      </c>
+      <c r="AD17" s="66" t="n">
+        <v>29.71674534693459</v>
+      </c>
+      <c r="AE17" s="67" t="n">
+        <v>18.33434113617269</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="57" t="inlineStr">
+        <is>
+          <t>Media One Hotel</t>
+        </is>
+      </c>
+      <c r="B18" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D18" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E18" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="61" t="n">
+        <v>264</v>
+      </c>
+      <c r="G18" s="62" t="n">
+        <v>1.715801886792453</v>
+      </c>
+      <c r="H18" s="59" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="I18" s="62" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="J18" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K18" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="63" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="M18" s="62" t="n">
+        <v>7.333333333333342</v>
+      </c>
+      <c r="N18" s="61" t="n">
+        <v>702</v>
+      </c>
+      <c r="O18" s="61" t="n">
+        <v>8</v>
+      </c>
+      <c r="P18" s="62" t="n">
+        <v>4.323902439024391</v>
+      </c>
+      <c r="Q18" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="R18" s="62" t="n">
+        <v>7</v>
+      </c>
+      <c r="S18" s="61" t="n">
+        <v>2008</v>
+      </c>
+      <c r="T18" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="U18" s="61" t="n">
+        <v>2018</v>
+      </c>
+      <c r="V18" s="62" t="n">
+        <v>3.055555555555556</v>
+      </c>
+      <c r="W18" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="64" t="n">
+        <v>37.45359321470574</v>
+      </c>
+      <c r="AC18" s="65" t="n">
+        <v>26.21751525029402</v>
+      </c>
+      <c r="AD18" s="66" t="n">
+        <v>26.21751525029402</v>
+      </c>
+      <c r="AE18" s="67" t="n">
+        <v>11.69846009153822</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="57" t="inlineStr">
+        <is>
+          <t>Staybridge Suites Dubai Internet City</t>
+        </is>
+      </c>
+      <c r="B19" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D19" s="58" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E19" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="61" t="n">
+        <v>225</v>
+      </c>
+      <c r="G19" s="62" t="n">
+        <v>1.025943396226415</v>
+      </c>
+      <c r="H19" s="59" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I19" s="62" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="J19" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K19" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="63" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="M19" s="62" t="n">
+        <v>8.000000000000005</v>
+      </c>
+      <c r="N19" s="61" t="n">
+        <v>227</v>
+      </c>
+      <c r="O19" s="61" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" s="62" t="n">
+        <v>1.304281842818428</v>
+      </c>
+      <c r="Q19" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="R19" s="62" t="n">
+        <v>1</v>
+      </c>
+      <c r="S19" s="61" t="n">
+        <v>2021</v>
+      </c>
+      <c r="T19" s="62" t="n">
+        <v>4.6875</v>
+      </c>
+      <c r="U19" s="61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="V19" s="62" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="W19" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="64" t="n">
+        <v>37.15105857237818</v>
+      </c>
+      <c r="AC19" s="65" t="n">
+        <v>26.00574100066473</v>
+      </c>
+      <c r="AD19" s="66" t="n">
+        <v>26.00574100066473</v>
+      </c>
+      <c r="AE19" s="67" t="n">
+        <v>11.29685496982706</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="57" t="inlineStr">
+        <is>
+          <t>Arjaan by Rotana - Dubai Media City</t>
+        </is>
+      </c>
+      <c r="B20" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="58" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="61" t="n">
+        <v>167</v>
+      </c>
+      <c r="G20" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="59" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="I20" s="62" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="J20" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K20" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="63" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="M20" s="62" t="n">
+        <v>4.000000000000005</v>
+      </c>
+      <c r="N20" s="61" t="n">
+        <v>562</v>
+      </c>
+      <c r="O20" s="61" t="n">
+        <v>19</v>
+      </c>
+      <c r="P20" s="62" t="n">
+        <v>5.476856368563686</v>
+      </c>
+      <c r="Q20" s="61" t="n">
+        <v>2</v>
+      </c>
+      <c r="R20" s="62" t="n">
+        <v>2</v>
+      </c>
+      <c r="S20" s="61" t="n">
+        <v>2008</v>
+      </c>
+      <c r="T20" s="62" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="U20" s="61" t="n">
+        <v>2017</v>
+      </c>
+      <c r="V20" s="62" t="n">
+        <v>2.777777777777778</v>
+      </c>
+      <c r="W20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="64" t="n">
+        <v>30.67963414634147</v>
+      </c>
+      <c r="AC20" s="65" t="n">
+        <v>21.47574390243903</v>
+      </c>
+      <c r="AD20" s="66" t="n">
+        <v>21.47574390243903</v>
+      </c>
+      <c r="AE20" s="67" t="n">
+        <v>2.706244736671905</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="57" t="inlineStr">
+        <is>
+          <t>Radisson Blu Media City</t>
+        </is>
+      </c>
+      <c r="B21" s="58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="59" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D21" s="58" t="inlineStr">
+        <is>
+          <t>R+S</t>
+        </is>
+      </c>
+      <c r="E21" s="60" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="61" t="n">
+        <v>246</v>
+      </c>
+      <c r="G21" s="62" t="n">
+        <v>1.397405660377358</v>
+      </c>
+      <c r="H21" s="59" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I21" s="62" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="J21" s="63" t="n">
+        <v>4</v>
+      </c>
+      <c r="K21" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="63" t="n">
+        <v>8</v>
+      </c>
+      <c r="M21" s="62" t="n">
+        <v>2</v>
+      </c>
+      <c r="N21" s="61" t="n">
+        <v>582</v>
+      </c>
+      <c r="O21" s="61" t="n">
+        <v>12</v>
+      </c>
+      <c r="P21" s="62" t="n">
+        <v>4.443577235772358</v>
+      </c>
+      <c r="Q21" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="R21" s="62" t="n">
+        <v>4</v>
+      </c>
+      <c r="S21" s="61" t="n">
+        <v>2006</v>
+      </c>
+      <c r="T21" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" s="61" t="n">
+        <v>2007</v>
+      </c>
+      <c r="V21" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="X21" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="64" t="n">
+        <v>28.64098289614972</v>
+      </c>
+      <c r="AC21" s="65" t="n">
+        <v>20.0486880273048</v>
+      </c>
+      <c r="AD21" s="66" t="n">
+        <v>20.0486880273048</v>
+      </c>
+      <c r="AE21" s="67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="39" t="inlineStr">
+        <is>
+          <t>SCORING METHODOLOGY (NO BRAND PENALTY):</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Total Keys:</t>
+        </is>
+      </c>
+      <c r="B25" s="56" t="inlineStr">
+        <is>
+          <t>Total rooms + suites + apartments - Max 15 pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Room Mix:</t>
+        </is>
+      </c>
+      <c r="B26" s="56" t="inlineStr">
+        <is>
+          <t>R+S+A = 3pts, Any 2 = 2pts, Any 1 = 1pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Distance:</t>
+        </is>
+      </c>
+      <c r="B27" s="56" t="inlineStr">
+        <is>
+          <t>Inverted - Closer = More Points - Max 20 pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  TripAdvisor &amp; Booking:</t>
+        </is>
+      </c>
+      <c r="B28" s="56" t="inlineStr">
+        <is>
+          <t>Normalized ratings - Max 10 pts each</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Meeting:</t>
+        </is>
+      </c>
+      <c r="B29" s="56" t="inlineStr">
+        <is>
+          <t>Space sqm (8pts) + Room count (4pts) = Max 12 pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  F&amp;B:</t>
+        </is>
+      </c>
+      <c r="B30" s="56" t="inlineStr">
+        <is>
+          <t>Restaurants + Bars - Normalized - Max 8 pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Opening Year:</t>
+        </is>
+      </c>
+      <c r="B31" s="56" t="inlineStr">
+        <is>
+          <t>Newer hotels get MORE points - Max 5 pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Renovation:</t>
+        </is>
+      </c>
+      <c r="B32" s="56" t="inlineStr">
+        <is>
+          <t>More recent renovation = MORE points - Max 5 pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Binary:</t>
+        </is>
+      </c>
+      <c r="B33" s="56" t="inlineStr">
+        <is>
+          <t>Pool, Gym, Spa, Sauna, Kids Club = 1pt each</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Star Multiplier:</t>
+        </is>
+      </c>
+      <c r="B34" s="56" t="inlineStr">
+        <is>
+          <t>5-star = 1.30 (+30%), 4-star = 0.70 (-30%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  NO PENALTIES:</t>
+        </is>
+      </c>
+      <c r="B35" s="56" t="inlineStr">
+        <is>
+          <t>Brand penalties REMOVED</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B25:G25"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
     <tabColor theme="1"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5114,7 +7394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>

</xml_diff>